<commit_message>
Load Diana stats from file
</commit_message>
<xml_diff>
--- a/Rpg.Client/BalanceConverter/Balance.xlsx
+++ b/Rpg.Client/BalanceConverter/Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\BalanceConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF12C6A-8AD6-449F-A854-AE33102534A8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507DCDBB-7C72-4130-8184-CE5E965FDD48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Berimir</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>SupportRank</t>
+  </si>
+  <si>
+    <t>Diana</t>
   </si>
 </sst>
 </file>
@@ -395,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB788DC-BDD6-4B96-9685-7F173364C01C}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,10 +441,10 @@
         <v>1</v>
       </c>
       <c r="B3">
+        <v>0.3</v>
+      </c>
+      <c r="C3">
         <v>0.7</v>
-      </c>
-      <c r="C3">
-        <v>0.3</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -459,6 +462,20 @@
       </c>
       <c r="D4">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0.8</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Draw last heroes on the title
</commit_message>
<xml_diff>
--- a/Rpg.Client/BalanceConverter/Balance.xlsx
+++ b/Rpg.Client/BalanceConverter/Balance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\BalanceConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507DCDBB-7C72-4130-8184-CE5E965FDD48}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C67D8C-F3E1-4B03-A906-BCCB43381C0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
   <si>
     <t>Berimir</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Diana</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Mode</t>
   </si>
 </sst>
 </file>
@@ -398,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB788DC-BDD6-4B96-9685-7F173364C01C}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -411,7 +420,7 @@
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -421,8 +430,14 @@
       <c r="D1" t="s">
         <v>5</v>
       </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -435,8 +450,11 @@
       <c r="D2">
         <v>0.1</v>
       </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -449,8 +467,11 @@
       <c r="D3">
         <v>0</v>
       </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -463,8 +484,11 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -476,6 +500,9 @@
       </c>
       <c r="D5">
         <v>0.2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
WIP Read basics from excel
</commit_message>
<xml_diff>
--- a/Rpg.Client/BalanceConverter/Balance.xlsx
+++ b/Rpg.Client/BalanceConverter/Balance.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\BalanceConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C67D8C-F3E1-4B03-A906-BCCB43381C0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6387E3C6-0463-4FC6-A8EF-769F00478228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
+    <sheet name="Basics" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Berimir</t>
   </si>
@@ -55,6 +56,30 @@
   </si>
   <si>
     <t>Mode</t>
+  </si>
+  <si>
+    <t>HITPOINTS_BASE</t>
+  </si>
+  <si>
+    <t>HITPOINTS_PER_LEVEL_BASE</t>
+  </si>
+  <si>
+    <t>ARMOR_BASE</t>
+  </si>
+  <si>
+    <t>DAMAGE_BASE</t>
+  </si>
+  <si>
+    <t>SUPPORT_BASE</t>
+  </si>
+  <si>
+    <t>HERO_POWER_MULTIPLICATOR</t>
+  </si>
+  <si>
+    <t>POWER_BASE</t>
+  </si>
+  <si>
+    <t>POWER_PER_LEVEL_BASE</t>
   </si>
 </sst>
 </file>
@@ -409,8 +434,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB788DC-BDD6-4B96-9685-7F173364C01C}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -508,4 +533,88 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B85002-EDF4-4A43-BEA6-7D3643547930}">
+  <dimension ref="A1:B8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <f>B1/10</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Store stats of the all heroes in the excel document
</commit_message>
<xml_diff>
--- a/Rpg.Client/BalanceConverter/Balance.xlsx
+++ b/Rpg.Client/BalanceConverter/Balance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PROJECTS\ewar\Rpg.Client\BalanceConverter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6387E3C6-0463-4FC6-A8EF-769F00478228}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8AB37CF-A295-4B2F-85A8-97517E5E41EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7FA6A51-E496-472E-BD03-21D5ADDBF1BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Units" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="26">
   <si>
     <t>Berimir</t>
   </si>
@@ -80,6 +80,30 @@
   </si>
   <si>
     <t>POWER_PER_LEVEL_BASE</t>
+  </si>
+  <si>
+    <t>Maosin</t>
+  </si>
+  <si>
+    <t>Ping</t>
+  </si>
+  <si>
+    <t>Cheng</t>
+  </si>
+  <si>
+    <t>Kakhotep</t>
+  </si>
+  <si>
+    <t>Amun</t>
+  </si>
+  <si>
+    <t>Leonidas</t>
+  </si>
+  <si>
+    <t>Nubiti</t>
+  </si>
+  <si>
+    <t>Geron</t>
   </si>
 </sst>
 </file>
@@ -432,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB788DC-BDD6-4B96-9685-7F173364C01C}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,13 +539,13 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>0.2</v>
       </c>
       <c r="C5">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="D5">
         <v>0.2</v>
@@ -530,8 +554,145 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6">
+        <v>0.8</v>
+      </c>
+      <c r="C6">
+        <v>0.1</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7">
+        <v>0.2</v>
+      </c>
+      <c r="C7">
+        <v>0.1</v>
+      </c>
+      <c r="D7">
+        <v>0.7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+      <c r="C8">
+        <v>0.9</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>0.1</v>
+      </c>
+      <c r="C9">
+        <v>0.8</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <v>0.2</v>
+      </c>
+      <c r="C10">
+        <v>0.1</v>
+      </c>
+      <c r="D10">
+        <v>0.7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11">
+        <v>0.5</v>
+      </c>
+      <c r="C11">
+        <v>0.4</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0.8</v>
+      </c>
+      <c r="D12">
+        <v>0.2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13">
+        <v>0.35</v>
+      </c>
+      <c r="C13">
+        <v>0.5</v>
+      </c>
+      <c r="D13">
+        <v>0.15</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -539,7 +700,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21B85002-EDF4-4A43-BEA6-7D3643547930}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>

</xml_diff>